<commit_message>
some more work on the report
</commit_message>
<xml_diff>
--- a/knowledgerep/Book1.xlsx
+++ b/knowledgerep/Book1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbhatta1\dev\ml\aima-python\knowledgerep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A931D346-81E4-4611-9E79-34A2D19DBCC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108DC80B-1A21-4DA7-AE17-DBEF69E44992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Probability of Evidence" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>AI</t>
   </si>
@@ -94,12 +96,81 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>ltgtmca</t>
+  </si>
+  <si>
+    <t>mcanot</t>
+  </si>
+  <si>
+    <t>notconform</t>
+  </si>
+  <si>
+    <t>ltgtmcanot</t>
+  </si>
+  <si>
+    <t>mcanotconform</t>
+  </si>
+  <si>
+    <t>ltgtmcanotconform</t>
+  </si>
+  <si>
+    <t>ltgt</t>
+  </si>
+  <si>
+    <t>mca</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>conform</t>
+  </si>
+  <si>
+    <t>ltgtmins</t>
+  </si>
+  <si>
+    <t>minsstop</t>
+  </si>
+  <si>
+    <t>stopsomewhere</t>
+  </si>
+  <si>
+    <t>somewherefirst</t>
+  </si>
+  <si>
+    <t>ltgtminsstop</t>
+  </si>
+  <si>
+    <t>minsstopsomewhere</t>
+  </si>
+  <si>
+    <t>stopsomewherefirst</t>
+  </si>
+  <si>
+    <t>ltgtminsstopsomewhere</t>
+  </si>
+  <si>
+    <t>minsstopsomewherefirst</t>
+  </si>
+  <si>
+    <t>ltgtminsstopsomewherefirst</t>
+  </si>
+  <si>
+    <t>mins</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Probability of Evidence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,12 +224,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -539,7 +611,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -575,7 +647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -642,7 +714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -709,10 +781,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -929,4 +1001,213 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FE8B21-C0B2-4895-AF9C-CE7E546CD8B6}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H40" sqref="H40:H41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>5.1633999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>3.8699999999999997E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>7.9094999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>3.8699999999999997E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>1.547E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>1.93E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22">
+        <v>9.6690000000000005E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308052E7-18AC-40B6-99C7-BFEC338FE06C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>